<commit_message>
Added demo for student registeration form
</commit_message>
<xml_diff>
--- a/studentdata.xlsx
+++ b/studentdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>stu_first_name</t>
   </si>
@@ -211,6 +211,24 @@
   </si>
   <si>
     <t>Jang Pura</t>
+  </si>
+  <si>
+    <t>Pulkit</t>
+  </si>
+  <si>
+    <t>Rahul Aggarwal</t>
+  </si>
+  <si>
+    <t>Aggarwal</t>
+  </si>
+  <si>
+    <t>Rajni Rahul Aggarwal</t>
+  </si>
+  <si>
+    <t>989 Bazar Sita Ram</t>
+  </si>
+  <si>
+    <t>Chawri Bazar</t>
   </si>
 </sst>
 </file>
@@ -542,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -687,7 +705,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C10" si="0">A4&amp;" "&amp;B4</f>
+        <f t="shared" ref="C4:C11" si="0">A4&amp;" "&amp;B4</f>
         <v>Rubeen Hatoon</v>
       </c>
       <c r="D4" t="s">
@@ -950,6 +968,45 @@
       </c>
       <c r="L10">
         <v>110042</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Pulkit Aggarwal</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>123354</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11">
+        <v>9213456859</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>110006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the functionality for marksheet uploading
</commit_message>
<xml_diff>
--- a/studentdata.xlsx
+++ b/studentdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="76">
   <si>
     <t>stu_first_name</t>
   </si>
@@ -229,6 +229,21 @@
   </si>
   <si>
     <t>Chawri Bazar</t>
+  </si>
+  <si>
+    <t>Shami</t>
+  </si>
+  <si>
+    <t>Amjad Khan</t>
+  </si>
+  <si>
+    <t>Ameena Khan</t>
+  </si>
+  <si>
+    <t>855 Kachla Baba</t>
+  </si>
+  <si>
+    <t>Lamdapur</t>
   </si>
 </sst>
 </file>
@@ -560,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A2" sqref="A2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -705,7 +720,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C11" si="0">A4&amp;" "&amp;B4</f>
+        <f>A4&amp;" "&amp;B4</f>
         <v>Rubeen Hatoon</v>
       </c>
       <c r="D4" t="s">
@@ -744,7 +759,7 @@
         <v>33</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>A5&amp;" "&amp;B5</f>
         <v>Rahul Sharma</v>
       </c>
       <c r="D5" t="s">
@@ -783,7 +798,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>A6&amp;" "&amp;B6</f>
         <v>Kajal Gupta</v>
       </c>
       <c r="D6" t="s">
@@ -822,7 +837,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f>A7&amp;" "&amp;B7</f>
         <v>Zubaida Khan</v>
       </c>
       <c r="D7" t="s">
@@ -861,7 +876,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f>A8&amp;" "&amp;B8</f>
         <v>Rajat Sharma</v>
       </c>
       <c r="D8" t="s">
@@ -900,7 +915,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f>A9&amp;" "&amp;B9</f>
         <v>Ankit Mishra</v>
       </c>
       <c r="D9" t="s">
@@ -939,7 +954,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f>A10&amp;" "&amp;B10</f>
         <v>Zoya Ahmad</v>
       </c>
       <c r="D10" t="s">
@@ -978,14 +993,14 @@
         <v>67</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f>A11&amp;" "&amp;B11</f>
         <v>Pulkit Aggarwal</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
       <c r="E11">
-        <v>123354</v>
+        <v>12354</v>
       </c>
       <c r="F11" t="s">
         <v>66</v>
@@ -1007,6 +1022,45 @@
       </c>
       <c r="L11">
         <v>110006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="str">
+        <f>A12&amp;" "&amp;B12</f>
+        <v>Shami Khan</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>12355</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12">
+        <v>9874123654</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12">
+        <v>110001</v>
       </c>
     </row>
   </sheetData>
@@ -1016,14 +1070,444 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection sqref="A1:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A1&amp;" "&amp;B1</f>
+        <v>Sultan Ahmad</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1">
+        <v>12345</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1">
+        <v>9654123123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1">
+        <v>110018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="str">
+        <f>A2&amp;" "&amp;B2</f>
+        <v>Kashif Khan</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>12346</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2">
+        <v>9652123123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>110006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="str">
+        <f>A3&amp;" "&amp;B3</f>
+        <v>Rubeen Hatoon</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>12347</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>9212392123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3">
+        <v>110041</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="str">
+        <f>A4&amp;" "&amp;B4</f>
+        <v>Rahul Sharma</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>12348</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>9658789789</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <v>110022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="str">
+        <f>A5&amp;" "&amp;B5</f>
+        <v>Kajal Gupta</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>12349</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>9632174589</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="str">
+        <f>A6&amp;" "&amp;B6</f>
+        <v>Zubaida Khan</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>12350</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6">
+        <v>9212654654</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6">
+        <v>110033</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="str">
+        <f>A7&amp;" "&amp;B7</f>
+        <v>Rajat Sharma</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>12351</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7">
+        <v>9632587417</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7">
+        <v>110045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="str">
+        <f>A8&amp;" "&amp;B8</f>
+        <v>Ankit Mishra</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>12352</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8">
+        <v>9685236514</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8">
+        <v>110025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="str">
+        <f>A9&amp;" "&amp;B9</f>
+        <v>Zoya Ahmad</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>12353</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9">
+        <v>9652123123</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9">
+        <v>110042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="str">
+        <f>A10&amp;" "&amp;B10</f>
+        <v>Pulkit Aggarwal</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>12354</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10">
+        <v>9213456859</v>
+      </c>
+      <c r="H10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10">
+        <v>110006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="str">
+        <f>A11&amp;" "&amp;B11</f>
+        <v>Shami Khan</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>12355</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11">
+        <v>9874123654</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>110001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>